<commit_message>
updated PPT results and TUGT code
</commit_message>
<xml_diff>
--- a/Results/Bayes_PPT_summary.xlsx
+++ b/Results/Bayes_PPT_summary.xlsx
@@ -416,31 +416,31 @@
         </is>
       </c>
       <c r="B2">
-        <v>-1.317</v>
+        <v>0.871</v>
       </c>
       <c r="C2">
-        <v>1.494</v>
+        <v>0.443</v>
       </c>
       <c r="D2">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="E2">
-        <v>0.008999999999999999</v>
+        <v>0.004</v>
       </c>
       <c r="F2">
-        <v>-4.268</v>
+        <v>-0.001</v>
       </c>
       <c r="G2">
-        <v>-2.298</v>
+        <v>0.577</v>
       </c>
       <c r="H2">
-        <v>-1.315</v>
+        <v>0.871</v>
       </c>
       <c r="I2">
-        <v>-0.334</v>
+        <v>1.166</v>
       </c>
       <c r="J2">
-        <v>1.628</v>
+        <v>1.741</v>
       </c>
     </row>
     <row r="3">
@@ -450,31 +450,31 @@
         </is>
       </c>
       <c r="B3">
-        <v>-1.163</v>
+        <v>0.673</v>
       </c>
       <c r="C3">
-        <v>1.494</v>
+        <v>0.439</v>
       </c>
       <c r="D3">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="E3">
-        <v>0.008999999999999999</v>
+        <v>0.004</v>
       </c>
       <c r="F3">
-        <v>-4.118</v>
+        <v>-0.191</v>
       </c>
       <c r="G3">
-        <v>-2.143</v>
+        <v>0.381</v>
       </c>
       <c r="H3">
-        <v>-1.163</v>
+        <v>0.674</v>
       </c>
       <c r="I3">
-        <v>-0.182</v>
+        <v>0.967</v>
       </c>
       <c r="J3">
-        <v>1.795</v>
+        <v>1.535</v>
       </c>
     </row>
     <row r="4">
@@ -484,31 +484,31 @@
         </is>
       </c>
       <c r="B4">
-        <v>-2.082</v>
+        <v>0.519</v>
       </c>
       <c r="C4">
-        <v>1.581</v>
+        <v>0.429</v>
       </c>
       <c r="D4">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="E4">
         <v>0.004</v>
       </c>
       <c r="F4">
-        <v>-5.198</v>
+        <v>-0.325</v>
       </c>
       <c r="G4">
-        <v>-3.124</v>
+        <v>0.234</v>
       </c>
       <c r="H4">
-        <v>-2.083</v>
+        <v>0.52</v>
       </c>
       <c r="I4">
-        <v>-1.039</v>
+        <v>0.805</v>
       </c>
       <c r="J4">
-        <v>1.037</v>
+        <v>1.358</v>
       </c>
     </row>
     <row r="5">
@@ -518,31 +518,31 @@
         </is>
       </c>
       <c r="B5">
-        <v>-1.263</v>
+        <v>0.872</v>
       </c>
       <c r="C5">
-        <v>1.495</v>
+        <v>0.48</v>
       </c>
       <c r="D5">
+        <v>0.001</v>
+      </c>
+      <c r="E5">
         <v>0.003</v>
       </c>
-      <c r="E5">
-        <v>0.008999999999999999</v>
-      </c>
       <c r="F5">
-        <v>-4.216</v>
+        <v>-0.074</v>
       </c>
       <c r="G5">
-        <v>-2.245</v>
+        <v>0.554</v>
       </c>
       <c r="H5">
-        <v>-1.264</v>
+        <v>0.873</v>
       </c>
       <c r="I5">
-        <v>-0.279</v>
+        <v>1.191</v>
       </c>
       <c r="J5">
-        <v>1.686</v>
+        <v>1.817</v>
       </c>
     </row>
     <row r="6">
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.8159999999999999</v>
+        <v>0.975</v>
       </c>
       <c r="C6">
-        <v>0.387</v>
+        <v>0.157</v>
       </c>
       <c r="D6">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -586,16 +586,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.788</v>
+        <v>0.9379999999999999</v>
       </c>
       <c r="C7">
-        <v>0.409</v>
+        <v>0.242</v>
       </c>
       <c r="D7">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -620,16 +620,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.909</v>
+        <v>0.887</v>
       </c>
       <c r="C8">
-        <v>0.288</v>
+        <v>0.316</v>
       </c>
       <c r="D8">
         <v>0.001</v>
       </c>
       <c r="E8">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -654,16 +654,16 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.806</v>
+        <v>0.965</v>
       </c>
       <c r="C9">
-        <v>0.396</v>
+        <v>0.183</v>
       </c>
       <c r="D9">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -688,22 +688,22 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.5590000000000001</v>
+        <v>0.869</v>
       </c>
       <c r="C10">
-        <v>0.496</v>
+        <v>0.338</v>
       </c>
       <c r="D10">
         <v>0.001</v>
       </c>
       <c r="E10">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.535</v>
+        <v>0.856</v>
       </c>
       <c r="C11">
-        <v>0.499</v>
+        <v>0.351</v>
       </c>
       <c r="D11">
         <v>0.001</v>
       </c>
       <c r="E11">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -756,16 +756,16 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.61</v>
+        <v>0.671</v>
       </c>
       <c r="C12">
-        <v>0.488</v>
+        <v>0.47</v>
       </c>
       <c r="D12">
         <v>0.001</v>
       </c>
       <c r="E12">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -790,22 +790,22 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.553</v>
+        <v>0.823</v>
       </c>
       <c r="C13">
-        <v>0.497</v>
+        <v>0.382</v>
       </c>
       <c r="D13">
         <v>0.001</v>
       </c>
       <c r="E13">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -824,22 +824,22 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.576</v>
+        <v>0.977</v>
       </c>
       <c r="C14">
-        <v>0.494</v>
+        <v>0.149</v>
       </c>
       <c r="D14">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -858,10 +858,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.552</v>
+        <v>0.821</v>
       </c>
       <c r="C15">
-        <v>0.497</v>
+        <v>0.383</v>
       </c>
       <c r="D15">
         <v>0.001</v>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -892,22 +892,22 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.619</v>
+        <v>0.872</v>
       </c>
       <c r="C16">
-        <v>0.486</v>
+        <v>0.334</v>
       </c>
       <c r="D16">
         <v>0.001</v>
       </c>
       <c r="E16">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -926,22 +926,22 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.5679999999999999</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="C17">
-        <v>0.495</v>
+        <v>0.247</v>
       </c>
       <c r="D17">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -960,22 +960,22 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.579</v>
+        <v>0.93</v>
       </c>
       <c r="C18">
-        <v>0.494</v>
+        <v>0.256</v>
       </c>
       <c r="D18">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -994,10 +994,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.551</v>
+        <v>0.852</v>
       </c>
       <c r="C19">
-        <v>0.497</v>
+        <v>0.355</v>
       </c>
       <c r="D19">
         <v>0.001</v>
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1028,22 +1028,22 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.611</v>
+        <v>0.836</v>
       </c>
       <c r="C20">
-        <v>0.488</v>
+        <v>0.37</v>
       </c>
       <c r="D20">
         <v>0.001</v>
       </c>
       <c r="E20">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1062,10 +1062,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.5679999999999999</v>
+        <v>0.758</v>
       </c>
       <c r="C21">
-        <v>0.495</v>
+        <v>0.428</v>
       </c>
       <c r="D21">
         <v>0.001</v>
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1096,16 +1096,16 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.539</v>
+        <v>0.48</v>
       </c>
       <c r="C22">
-        <v>0.498</v>
+        <v>0.5</v>
       </c>
       <c r="D22">
         <v>0.001</v>
       </c>
       <c r="E22">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1130,16 +1130,16 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.513</v>
+        <v>0.73</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0.444</v>
       </c>
       <c r="D23">
         <v>0.001</v>
       </c>
       <c r="E23">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1164,16 +1164,16 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.604</v>
+        <v>0.553</v>
       </c>
       <c r="C24">
-        <v>0.489</v>
+        <v>0.497</v>
       </c>
       <c r="D24">
         <v>0.001</v>
       </c>
       <c r="E24">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1198,16 +1198,16 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.528</v>
+        <v>0.569</v>
       </c>
       <c r="C25">
-        <v>0.499</v>
+        <v>0.495</v>
       </c>
       <c r="D25">
         <v>0.001</v>
       </c>
       <c r="E25">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1232,10 +1232,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.575</v>
+        <v>0.872</v>
       </c>
       <c r="C26">
-        <v>0.494</v>
+        <v>0.335</v>
       </c>
       <c r="D26">
         <v>0.001</v>
@@ -1247,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1266,22 +1266,22 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.547</v>
+        <v>0.896</v>
       </c>
       <c r="C27">
-        <v>0.498</v>
+        <v>0.306</v>
       </c>
       <c r="D27">
         <v>0.001</v>
       </c>
       <c r="E27">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1300,22 +1300,22 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.744</v>
+        <v>0.894</v>
       </c>
       <c r="C28">
-        <v>0.436</v>
+        <v>0.308</v>
       </c>
       <c r="D28">
         <v>0.001</v>
       </c>
       <c r="E28">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1334,22 +1334,22 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.5669999999999999</v>
+        <v>0.883</v>
       </c>
       <c r="C29">
-        <v>0.496</v>
+        <v>0.322</v>
       </c>
       <c r="D29">
         <v>0.001</v>
       </c>
       <c r="E29">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1368,19 +1368,19 @@
         </is>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.39</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1402,22 +1402,22 @@
         </is>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0.578</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>0.494</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1436,22 +1436,22 @@
         </is>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1470,25 +1470,25 @@
         </is>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0.494</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1504,22 +1504,22 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.552</v>
+        <v>0.841</v>
       </c>
       <c r="C34">
-        <v>0.497</v>
+        <v>0.366</v>
       </c>
       <c r="D34">
         <v>0.001</v>
       </c>
       <c r="E34">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1538,22 +1538,22 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.523</v>
+        <v>0.89</v>
       </c>
       <c r="C35">
-        <v>0.499</v>
+        <v>0.313</v>
       </c>
       <c r="D35">
         <v>0.001</v>
       </c>
       <c r="E35">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -1572,16 +1572,16 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.964</v>
+        <v>0.759</v>
       </c>
       <c r="C36">
-        <v>0.187</v>
+        <v>0.428</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="E36">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1606,22 +1606,22 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.542</v>
+        <v>0.917</v>
       </c>
       <c r="C37">
-        <v>0.498</v>
+        <v>0.275</v>
       </c>
       <c r="D37">
         <v>0.001</v>
       </c>
       <c r="E37">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -1640,22 +1640,22 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.515</v>
+        <v>0.892</v>
       </c>
       <c r="C38">
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="D38">
         <v>0.001</v>
       </c>
       <c r="E38">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -1674,10 +1674,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.492</v>
+        <v>0.799</v>
       </c>
       <c r="C39">
-        <v>0.5</v>
+        <v>0.401</v>
       </c>
       <c r="D39">
         <v>0.001</v>
@@ -1689,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -1708,22 +1708,22 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.59</v>
+        <v>0.76</v>
       </c>
       <c r="C40">
-        <v>0.492</v>
+        <v>0.427</v>
       </c>
       <c r="D40">
         <v>0.001</v>
       </c>
       <c r="E40">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -1742,22 +1742,22 @@
         </is>
       </c>
       <c r="B41">
-        <v>0.508</v>
+        <v>0.957</v>
       </c>
       <c r="C41">
-        <v>0.5</v>
+        <v>0.202</v>
       </c>
       <c r="D41">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -1776,10 +1776,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.507</v>
+        <v>0.855</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>0.353</v>
       </c>
       <c r="D42">
         <v>0.001</v>
@@ -1791,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -1810,25 +1810,25 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.481</v>
+        <v>0.92</v>
       </c>
       <c r="C43">
-        <v>0.5</v>
+        <v>0.271</v>
       </c>
       <c r="D43">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -1844,22 +1844,22 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.582</v>
+        <v>0.887</v>
       </c>
       <c r="C44">
-        <v>0.493</v>
+        <v>0.317</v>
       </c>
       <c r="D44">
         <v>0.001</v>
       </c>
       <c r="E44">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -1878,25 +1878,25 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.498</v>
+        <v>0.97</v>
       </c>
       <c r="C45">
-        <v>0.5</v>
+        <v>0.172</v>
       </c>
       <c r="D45">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <v>1</v>
@@ -1912,10 +1912,10 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.439</v>
+        <v>0.779</v>
       </c>
       <c r="C46">
-        <v>0.496</v>
+        <v>0.415</v>
       </c>
       <c r="D46">
         <v>0.001</v>
@@ -1927,10 +1927,10 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -1946,10 +1946,10 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.409</v>
+        <v>0.822</v>
       </c>
       <c r="C47">
-        <v>0.492</v>
+        <v>0.382</v>
       </c>
       <c r="D47">
         <v>0.001</v>
@@ -1961,10 +1961,10 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -1980,22 +1980,22 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.522</v>
+        <v>0.764</v>
       </c>
       <c r="C48">
-        <v>0.499</v>
+        <v>0.425</v>
       </c>
       <c r="D48">
         <v>0.001</v>
       </c>
       <c r="E48">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -2014,25 +2014,25 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.424</v>
+        <v>0.865</v>
       </c>
       <c r="C49">
-        <v>0.494</v>
+        <v>0.342</v>
       </c>
       <c r="D49">
         <v>0.001</v>
       </c>
       <c r="E49">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -2048,22 +2048,22 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.5649999999999999</v>
+        <v>0.914</v>
       </c>
       <c r="C50">
-        <v>0.496</v>
+        <v>0.281</v>
       </c>
       <c r="D50">
         <v>0.001</v>
       </c>
       <c r="E50">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -2082,22 +2082,22 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.539</v>
+        <v>0.901</v>
       </c>
       <c r="C51">
-        <v>0.498</v>
+        <v>0.299</v>
       </c>
       <c r="D51">
         <v>0.001</v>
       </c>
       <c r="E51">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -2116,22 +2116,22 @@
         </is>
       </c>
       <c r="B52">
-        <v>0.605</v>
+        <v>0.784</v>
       </c>
       <c r="C52">
-        <v>0.489</v>
+        <v>0.412</v>
       </c>
       <c r="D52">
         <v>0.001</v>
       </c>
       <c r="E52">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -2150,22 +2150,22 @@
         </is>
       </c>
       <c r="B53">
-        <v>0.5570000000000001</v>
+        <v>0.845</v>
       </c>
       <c r="C53">
-        <v>0.497</v>
+        <v>0.362</v>
       </c>
       <c r="D53">
         <v>0.001</v>
       </c>
       <c r="E53">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F53">
         <v>0</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -2184,22 +2184,22 @@
         </is>
       </c>
       <c r="B54">
-        <v>0.532</v>
+        <v>0.87</v>
       </c>
       <c r="C54">
-        <v>0.499</v>
+        <v>0.337</v>
       </c>
       <c r="D54">
         <v>0.001</v>
       </c>
       <c r="E54">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F54">
         <v>0</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -2218,10 +2218,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>0.506</v>
+        <v>0.764</v>
       </c>
       <c r="C55">
-        <v>0.5</v>
+        <v>0.424</v>
       </c>
       <c r="D55">
         <v>0.001</v>
@@ -2233,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -2252,16 +2252,16 @@
         </is>
       </c>
       <c r="B56">
-        <v>0.582</v>
+        <v>0.724</v>
       </c>
       <c r="C56">
-        <v>0.493</v>
+        <v>0.447</v>
       </c>
       <c r="D56">
         <v>0.001</v>
       </c>
       <c r="E56">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -2286,22 +2286,22 @@
         </is>
       </c>
       <c r="B57">
-        <v>0.524</v>
+        <v>0.907</v>
       </c>
       <c r="C57">
-        <v>0.499</v>
+        <v>0.291</v>
       </c>
       <c r="D57">
         <v>0.001</v>
       </c>
       <c r="E57">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -2320,22 +2320,22 @@
         </is>
       </c>
       <c r="B58">
-        <v>0.549</v>
+        <v>0.87</v>
       </c>
       <c r="C58">
-        <v>0.498</v>
+        <v>0.337</v>
       </c>
       <c r="D58">
         <v>0.001</v>
       </c>
       <c r="E58">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -2354,10 +2354,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>0.52</v>
+        <v>0.799</v>
       </c>
       <c r="C59">
-        <v>0.5</v>
+        <v>0.401</v>
       </c>
       <c r="D59">
         <v>0.001</v>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -2388,22 +2388,22 @@
         </is>
       </c>
       <c r="B60">
-        <v>0.606</v>
+        <v>0.835</v>
       </c>
       <c r="C60">
-        <v>0.489</v>
+        <v>0.371</v>
       </c>
       <c r="D60">
         <v>0.001</v>
       </c>
       <c r="E60">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -2422,22 +2422,22 @@
         </is>
       </c>
       <c r="B61">
-        <v>0.536</v>
+        <v>0.953</v>
       </c>
       <c r="C61">
-        <v>0.499</v>
+        <v>0.211</v>
       </c>
       <c r="D61">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -2456,16 +2456,16 @@
         </is>
       </c>
       <c r="B62">
-        <v>0.549</v>
+        <v>0.668</v>
       </c>
       <c r="C62">
-        <v>0.498</v>
+        <v>0.471</v>
       </c>
       <c r="D62">
         <v>0.001</v>
       </c>
       <c r="E62">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -2490,16 +2490,16 @@
         </is>
       </c>
       <c r="B63">
-        <v>0.521</v>
+        <v>0.651</v>
       </c>
       <c r="C63">
-        <v>0.5</v>
+        <v>0.477</v>
       </c>
       <c r="D63">
         <v>0.001</v>
       </c>
       <c r="E63">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2524,16 +2524,16 @@
         </is>
       </c>
       <c r="B64">
-        <v>0.596</v>
+        <v>0.636</v>
       </c>
       <c r="C64">
-        <v>0.491</v>
+        <v>0.481</v>
       </c>
       <c r="D64">
         <v>0.001</v>
       </c>
       <c r="E64">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2558,16 +2558,16 @@
         </is>
       </c>
       <c r="B65">
-        <v>0.541</v>
+        <v>0.368</v>
       </c>
       <c r="C65">
-        <v>0.498</v>
+        <v>0.482</v>
       </c>
       <c r="D65">
         <v>0.001</v>
       </c>
       <c r="E65">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -2592,10 +2592,10 @@
         </is>
       </c>
       <c r="B66">
-        <v>0.532</v>
+        <v>0.745</v>
       </c>
       <c r="C66">
-        <v>0.499</v>
+        <v>0.436</v>
       </c>
       <c r="D66">
         <v>0.001</v>
@@ -2626,10 +2626,10 @@
         </is>
       </c>
       <c r="B67">
-        <v>0.504</v>
+        <v>0.751</v>
       </c>
       <c r="C67">
-        <v>0.5</v>
+        <v>0.432</v>
       </c>
       <c r="D67">
         <v>0.001</v>
@@ -2641,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -2660,16 +2660,16 @@
         </is>
       </c>
       <c r="B68">
-        <v>0.579</v>
+        <v>0.585</v>
       </c>
       <c r="C68">
-        <v>0.494</v>
+        <v>0.493</v>
       </c>
       <c r="D68">
         <v>0.001</v>
       </c>
       <c r="E68">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -2694,22 +2694,22 @@
         </is>
       </c>
       <c r="B69">
-        <v>0.521</v>
+        <v>0.912</v>
       </c>
       <c r="C69">
-        <v>0.5</v>
+        <v>0.283</v>
       </c>
       <c r="D69">
         <v>0.001</v>
       </c>
       <c r="E69">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -2728,22 +2728,22 @@
         </is>
       </c>
       <c r="B70">
-        <v>0.569</v>
+        <v>0.928</v>
       </c>
       <c r="C70">
-        <v>0.495</v>
+        <v>0.258</v>
       </c>
       <c r="D70">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -2762,10 +2762,10 @@
         </is>
       </c>
       <c r="B71">
-        <v>0.545</v>
+        <v>0.794</v>
       </c>
       <c r="C71">
-        <v>0.498</v>
+        <v>0.404</v>
       </c>
       <c r="D71">
         <v>0.001</v>
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -2796,16 +2796,16 @@
         </is>
       </c>
       <c r="B72">
-        <v>0.616</v>
+        <v>0.72</v>
       </c>
       <c r="C72">
-        <v>0.486</v>
+        <v>0.449</v>
       </c>
       <c r="D72">
         <v>0.001</v>
       </c>
       <c r="E72">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -2830,22 +2830,22 @@
         </is>
       </c>
       <c r="B73">
-        <v>0.5620000000000001</v>
+        <v>0.866</v>
       </c>
       <c r="C73">
-        <v>0.496</v>
+        <v>0.341</v>
       </c>
       <c r="D73">
         <v>0.001</v>
       </c>
       <c r="E73">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -2864,22 +2864,22 @@
         </is>
       </c>
       <c r="B74">
-        <v>0.528</v>
+        <v>0.963</v>
       </c>
       <c r="C74">
-        <v>0.499</v>
+        <v>0.19</v>
       </c>
       <c r="D74">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F74">
         <v>0</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -2898,22 +2898,22 @@
         </is>
       </c>
       <c r="B75">
-        <v>0.503</v>
+        <v>0.801</v>
       </c>
       <c r="C75">
-        <v>0.5</v>
+        <v>0.399</v>
       </c>
       <c r="D75">
         <v>0.001</v>
       </c>
       <c r="E75">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F75">
         <v>0</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -2932,22 +2932,22 @@
         </is>
       </c>
       <c r="B76">
-        <v>0.603</v>
+        <v>0.908</v>
       </c>
       <c r="C76">
-        <v>0.489</v>
+        <v>0.289</v>
       </c>
       <c r="D76">
         <v>0.001</v>
       </c>
       <c r="E76">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -2966,10 +2966,10 @@
         </is>
       </c>
       <c r="B77">
-        <v>0.519</v>
+        <v>0.802</v>
       </c>
       <c r="C77">
-        <v>0.5</v>
+        <v>0.398</v>
       </c>
       <c r="D77">
         <v>0.001</v>
@@ -2981,7 +2981,7 @@
         <v>0</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -3000,10 +3000,10 @@
         </is>
       </c>
       <c r="B78">
-        <v>0.5659999999999999</v>
+        <v>0.742</v>
       </c>
       <c r="C78">
-        <v>0.496</v>
+        <v>0.438</v>
       </c>
       <c r="D78">
         <v>0.001</v>
@@ -3034,16 +3034,16 @@
         </is>
       </c>
       <c r="B79">
-        <v>0.543</v>
+        <v>0.615</v>
       </c>
       <c r="C79">
-        <v>0.498</v>
+        <v>0.487</v>
       </c>
       <c r="D79">
         <v>0.001</v>
       </c>
       <c r="E79">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3068,16 +3068,16 @@
         </is>
       </c>
       <c r="B80">
-        <v>0.606</v>
+        <v>0.616</v>
       </c>
       <c r="C80">
-        <v>0.489</v>
+        <v>0.486</v>
       </c>
       <c r="D80">
         <v>0.001</v>
       </c>
       <c r="E80">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -3102,16 +3102,16 @@
         </is>
       </c>
       <c r="B81">
-        <v>0.5570000000000001</v>
+        <v>0.429</v>
       </c>
       <c r="C81">
-        <v>0.497</v>
+        <v>0.495</v>
       </c>
       <c r="D81">
         <v>0.001</v>
       </c>
       <c r="E81">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81">
         <v>1</v>
@@ -3136,22 +3136,22 @@
         </is>
       </c>
       <c r="B82">
-        <v>0.57</v>
+        <v>0.931</v>
       </c>
       <c r="C82">
-        <v>0.495</v>
+        <v>0.254</v>
       </c>
       <c r="D82">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F82">
         <v>0</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -3170,22 +3170,22 @@
         </is>
       </c>
       <c r="B83">
-        <v>0.545</v>
+        <v>0.88</v>
       </c>
       <c r="C83">
-        <v>0.498</v>
+        <v>0.325</v>
       </c>
       <c r="D83">
         <v>0.001</v>
       </c>
       <c r="E83">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="F83">
         <v>0</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -3204,22 +3204,22 @@
         </is>
       </c>
       <c r="B84">
-        <v>0.601</v>
+        <v>0.877</v>
       </c>
       <c r="C84">
-        <v>0.49</v>
+        <v>0.329</v>
       </c>
       <c r="D84">
         <v>0.001</v>
       </c>
       <c r="E84">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="F84">
         <v>0</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -3238,10 +3238,10 @@
         </is>
       </c>
       <c r="B85">
-        <v>0.5620000000000001</v>
+        <v>0.731</v>
       </c>
       <c r="C85">
-        <v>0.496</v>
+        <v>0.444</v>
       </c>
       <c r="D85">
         <v>0.001</v>
@@ -3272,10 +3272,10 @@
         </is>
       </c>
       <c r="B86">
-        <v>0.529</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="C86">
-        <v>0.499</v>
+        <v>0.39</v>
       </c>
       <c r="D86">
         <v>0.001</v>
@@ -3287,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -3306,10 +3306,10 @@
         </is>
       </c>
       <c r="B87">
-        <v>0.504</v>
+        <v>0.73</v>
       </c>
       <c r="C87">
-        <v>0.5</v>
+        <v>0.444</v>
       </c>
       <c r="D87">
         <v>0.001</v>
@@ -3340,16 +3340,16 @@
         </is>
       </c>
       <c r="B88">
-        <v>0.574</v>
+        <v>0.697</v>
       </c>
       <c r="C88">
-        <v>0.495</v>
+        <v>0.46</v>
       </c>
       <c r="D88">
         <v>0.001</v>
       </c>
       <c r="E88">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -3374,10 +3374,10 @@
         </is>
       </c>
       <c r="B89">
-        <v>0.52</v>
+        <v>0.636</v>
       </c>
       <c r="C89">
-        <v>0.5</v>
+        <v>0.481</v>
       </c>
       <c r="D89">
         <v>0.001</v>

</xml_diff>